<commit_message>
approved by tech lead :>
</commit_message>
<xml_diff>
--- a/SimpCity US2 & 16 Test Cases (NOT CHECKED BY THE TEAM).xlsx
+++ b/SimpCity US2 & 16 Test Cases (NOT CHECKED BY THE TEAM).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huiyi\Downloads\Year 3-Poly\Sem 3.2 DevOps\Test Cases (Not Checked)\Sprin 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claris Toh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E1E8F-E923-47E1-9616-419CBB80EE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E0EB6D-792A-4F78-9C1B-E9E9CA074ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="3960" windowWidth="21600" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US2 Sprint 5" sheetId="22" r:id="rId1"/>
@@ -1045,32 +1045,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,7 +1389,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,10 +1408,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="107"/>
+      <c r="C1" s="103"/>
       <c r="D1" s="40"/>
       <c r="E1" s="38"/>
       <c r="F1" s="42"/>
@@ -1424,24 +1424,24 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="99"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="100" t="s">
+      <c r="E2" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="99"/>
+      <c r="F2" s="105"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="99"/>
-      <c r="J2" s="100" t="s">
+      <c r="I2" s="105"/>
+      <c r="J2" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="101"/>
+      <c r="K2" s="106"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.25">
@@ -1554,20 +1554,20 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="102"/>
+      <c r="C7" s="107"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="102"/>
+      <c r="F7" s="107"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="102" t="s">
+      <c r="H7" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="102"/>
+      <c r="I7" s="107"/>
       <c r="J7"/>
       <c r="L7" s="4"/>
     </row>
@@ -1577,7 +1577,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="62" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="63" t="s">
@@ -1698,20 +1698,20 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="97" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="103">
+      <c r="A14" s="99">
         <v>1</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="106" t="s">
+      <c r="D14" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
       <c r="G14" s="94"/>
       <c r="H14" s="94"/>
       <c r="I14" s="94"/>
@@ -1719,9 +1719,9 @@
       <c r="K14" s="95"/>
     </row>
     <row r="15" spans="1:12" s="91" customFormat="1" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="103"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="105"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="101"/>
       <c r="D15" s="92" t="s">
         <v>48</v>
       </c>
@@ -1892,6 +1892,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
@@ -1899,11 +1904,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15:J17 G15:H17" xr:uid="{FCCE161A-7504-4579-B4D0-81456406B484}">

</xml_diff>